<commit_message>
Updates to include new notebook
</commit_message>
<xml_diff>
--- a/Gephi/Transform_To_DSG.xlsx
+++ b/Gephi/Transform_To_DSG.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougneedham\Documents\DMZ\Gephi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dneedham\Documents\DMZ\DMZ_2018\Gephi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A9F6B94-A8CF-4E0F-B760-53888642DCC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{5FA7DC29-6260-40B9-82DD-D8D953F85329}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BusMatrix" sheetId="1" r:id="rId1"/>
@@ -350,7 +349,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -637,6 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -664,7 +664,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,342 +977,342 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3986F226-D9D2-4973-9538-554C5DF7C3CD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="10" width="3.28515625" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" customWidth="1"/>
-    <col min="12" max="24" width="3.28515625" customWidth="1"/>
-    <col min="233" max="233" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="10" width="3.33203125" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" customWidth="1"/>
+    <col min="12" max="24" width="3.33203125" customWidth="1"/>
+    <col min="233" max="233" width="20.5546875" customWidth="1"/>
     <col min="234" max="237" width="0" hidden="1" customWidth="1"/>
-    <col min="238" max="242" width="3.28515625" customWidth="1"/>
-    <col min="243" max="243" width="4.28515625" customWidth="1"/>
-    <col min="244" max="280" width="3.28515625" customWidth="1"/>
-    <col min="489" max="489" width="20.5703125" customWidth="1"/>
+    <col min="238" max="242" width="3.33203125" customWidth="1"/>
+    <col min="243" max="243" width="4.33203125" customWidth="1"/>
+    <col min="244" max="280" width="3.33203125" customWidth="1"/>
+    <col min="489" max="489" width="20.5546875" customWidth="1"/>
     <col min="490" max="493" width="0" hidden="1" customWidth="1"/>
-    <col min="494" max="498" width="3.28515625" customWidth="1"/>
-    <col min="499" max="499" width="4.28515625" customWidth="1"/>
-    <col min="500" max="536" width="3.28515625" customWidth="1"/>
-    <col min="745" max="745" width="20.5703125" customWidth="1"/>
+    <col min="494" max="498" width="3.33203125" customWidth="1"/>
+    <col min="499" max="499" width="4.33203125" customWidth="1"/>
+    <col min="500" max="536" width="3.33203125" customWidth="1"/>
+    <col min="745" max="745" width="20.5546875" customWidth="1"/>
     <col min="746" max="749" width="0" hidden="1" customWidth="1"/>
-    <col min="750" max="754" width="3.28515625" customWidth="1"/>
-    <col min="755" max="755" width="4.28515625" customWidth="1"/>
-    <col min="756" max="792" width="3.28515625" customWidth="1"/>
-    <col min="1001" max="1001" width="20.5703125" customWidth="1"/>
+    <col min="750" max="754" width="3.33203125" customWidth="1"/>
+    <col min="755" max="755" width="4.33203125" customWidth="1"/>
+    <col min="756" max="792" width="3.33203125" customWidth="1"/>
+    <col min="1001" max="1001" width="20.5546875" customWidth="1"/>
     <col min="1002" max="1005" width="0" hidden="1" customWidth="1"/>
-    <col min="1006" max="1010" width="3.28515625" customWidth="1"/>
-    <col min="1011" max="1011" width="4.28515625" customWidth="1"/>
-    <col min="1012" max="1048" width="3.28515625" customWidth="1"/>
-    <col min="1257" max="1257" width="20.5703125" customWidth="1"/>
+    <col min="1006" max="1010" width="3.33203125" customWidth="1"/>
+    <col min="1011" max="1011" width="4.33203125" customWidth="1"/>
+    <col min="1012" max="1048" width="3.33203125" customWidth="1"/>
+    <col min="1257" max="1257" width="20.5546875" customWidth="1"/>
     <col min="1258" max="1261" width="0" hidden="1" customWidth="1"/>
-    <col min="1262" max="1266" width="3.28515625" customWidth="1"/>
-    <col min="1267" max="1267" width="4.28515625" customWidth="1"/>
-    <col min="1268" max="1304" width="3.28515625" customWidth="1"/>
-    <col min="1513" max="1513" width="20.5703125" customWidth="1"/>
+    <col min="1262" max="1266" width="3.33203125" customWidth="1"/>
+    <col min="1267" max="1267" width="4.33203125" customWidth="1"/>
+    <col min="1268" max="1304" width="3.33203125" customWidth="1"/>
+    <col min="1513" max="1513" width="20.5546875" customWidth="1"/>
     <col min="1514" max="1517" width="0" hidden="1" customWidth="1"/>
-    <col min="1518" max="1522" width="3.28515625" customWidth="1"/>
-    <col min="1523" max="1523" width="4.28515625" customWidth="1"/>
-    <col min="1524" max="1560" width="3.28515625" customWidth="1"/>
-    <col min="1769" max="1769" width="20.5703125" customWidth="1"/>
+    <col min="1518" max="1522" width="3.33203125" customWidth="1"/>
+    <col min="1523" max="1523" width="4.33203125" customWidth="1"/>
+    <col min="1524" max="1560" width="3.33203125" customWidth="1"/>
+    <col min="1769" max="1769" width="20.5546875" customWidth="1"/>
     <col min="1770" max="1773" width="0" hidden="1" customWidth="1"/>
-    <col min="1774" max="1778" width="3.28515625" customWidth="1"/>
-    <col min="1779" max="1779" width="4.28515625" customWidth="1"/>
-    <col min="1780" max="1816" width="3.28515625" customWidth="1"/>
-    <col min="2025" max="2025" width="20.5703125" customWidth="1"/>
+    <col min="1774" max="1778" width="3.33203125" customWidth="1"/>
+    <col min="1779" max="1779" width="4.33203125" customWidth="1"/>
+    <col min="1780" max="1816" width="3.33203125" customWidth="1"/>
+    <col min="2025" max="2025" width="20.5546875" customWidth="1"/>
     <col min="2026" max="2029" width="0" hidden="1" customWidth="1"/>
-    <col min="2030" max="2034" width="3.28515625" customWidth="1"/>
-    <col min="2035" max="2035" width="4.28515625" customWidth="1"/>
-    <col min="2036" max="2072" width="3.28515625" customWidth="1"/>
-    <col min="2281" max="2281" width="20.5703125" customWidth="1"/>
+    <col min="2030" max="2034" width="3.33203125" customWidth="1"/>
+    <col min="2035" max="2035" width="4.33203125" customWidth="1"/>
+    <col min="2036" max="2072" width="3.33203125" customWidth="1"/>
+    <col min="2281" max="2281" width="20.5546875" customWidth="1"/>
     <col min="2282" max="2285" width="0" hidden="1" customWidth="1"/>
-    <col min="2286" max="2290" width="3.28515625" customWidth="1"/>
-    <col min="2291" max="2291" width="4.28515625" customWidth="1"/>
-    <col min="2292" max="2328" width="3.28515625" customWidth="1"/>
-    <col min="2537" max="2537" width="20.5703125" customWidth="1"/>
+    <col min="2286" max="2290" width="3.33203125" customWidth="1"/>
+    <col min="2291" max="2291" width="4.33203125" customWidth="1"/>
+    <col min="2292" max="2328" width="3.33203125" customWidth="1"/>
+    <col min="2537" max="2537" width="20.5546875" customWidth="1"/>
     <col min="2538" max="2541" width="0" hidden="1" customWidth="1"/>
-    <col min="2542" max="2546" width="3.28515625" customWidth="1"/>
-    <col min="2547" max="2547" width="4.28515625" customWidth="1"/>
-    <col min="2548" max="2584" width="3.28515625" customWidth="1"/>
-    <col min="2793" max="2793" width="20.5703125" customWidth="1"/>
+    <col min="2542" max="2546" width="3.33203125" customWidth="1"/>
+    <col min="2547" max="2547" width="4.33203125" customWidth="1"/>
+    <col min="2548" max="2584" width="3.33203125" customWidth="1"/>
+    <col min="2793" max="2793" width="20.5546875" customWidth="1"/>
     <col min="2794" max="2797" width="0" hidden="1" customWidth="1"/>
-    <col min="2798" max="2802" width="3.28515625" customWidth="1"/>
-    <col min="2803" max="2803" width="4.28515625" customWidth="1"/>
-    <col min="2804" max="2840" width="3.28515625" customWidth="1"/>
-    <col min="3049" max="3049" width="20.5703125" customWidth="1"/>
+    <col min="2798" max="2802" width="3.33203125" customWidth="1"/>
+    <col min="2803" max="2803" width="4.33203125" customWidth="1"/>
+    <col min="2804" max="2840" width="3.33203125" customWidth="1"/>
+    <col min="3049" max="3049" width="20.5546875" customWidth="1"/>
     <col min="3050" max="3053" width="0" hidden="1" customWidth="1"/>
-    <col min="3054" max="3058" width="3.28515625" customWidth="1"/>
-    <col min="3059" max="3059" width="4.28515625" customWidth="1"/>
-    <col min="3060" max="3096" width="3.28515625" customWidth="1"/>
-    <col min="3305" max="3305" width="20.5703125" customWidth="1"/>
+    <col min="3054" max="3058" width="3.33203125" customWidth="1"/>
+    <col min="3059" max="3059" width="4.33203125" customWidth="1"/>
+    <col min="3060" max="3096" width="3.33203125" customWidth="1"/>
+    <col min="3305" max="3305" width="20.5546875" customWidth="1"/>
     <col min="3306" max="3309" width="0" hidden="1" customWidth="1"/>
-    <col min="3310" max="3314" width="3.28515625" customWidth="1"/>
-    <col min="3315" max="3315" width="4.28515625" customWidth="1"/>
-    <col min="3316" max="3352" width="3.28515625" customWidth="1"/>
-    <col min="3561" max="3561" width="20.5703125" customWidth="1"/>
+    <col min="3310" max="3314" width="3.33203125" customWidth="1"/>
+    <col min="3315" max="3315" width="4.33203125" customWidth="1"/>
+    <col min="3316" max="3352" width="3.33203125" customWidth="1"/>
+    <col min="3561" max="3561" width="20.5546875" customWidth="1"/>
     <col min="3562" max="3565" width="0" hidden="1" customWidth="1"/>
-    <col min="3566" max="3570" width="3.28515625" customWidth="1"/>
-    <col min="3571" max="3571" width="4.28515625" customWidth="1"/>
-    <col min="3572" max="3608" width="3.28515625" customWidth="1"/>
-    <col min="3817" max="3817" width="20.5703125" customWidth="1"/>
+    <col min="3566" max="3570" width="3.33203125" customWidth="1"/>
+    <col min="3571" max="3571" width="4.33203125" customWidth="1"/>
+    <col min="3572" max="3608" width="3.33203125" customWidth="1"/>
+    <col min="3817" max="3817" width="20.5546875" customWidth="1"/>
     <col min="3818" max="3821" width="0" hidden="1" customWidth="1"/>
-    <col min="3822" max="3826" width="3.28515625" customWidth="1"/>
-    <col min="3827" max="3827" width="4.28515625" customWidth="1"/>
-    <col min="3828" max="3864" width="3.28515625" customWidth="1"/>
-    <col min="4073" max="4073" width="20.5703125" customWidth="1"/>
+    <col min="3822" max="3826" width="3.33203125" customWidth="1"/>
+    <col min="3827" max="3827" width="4.33203125" customWidth="1"/>
+    <col min="3828" max="3864" width="3.33203125" customWidth="1"/>
+    <col min="4073" max="4073" width="20.5546875" customWidth="1"/>
     <col min="4074" max="4077" width="0" hidden="1" customWidth="1"/>
-    <col min="4078" max="4082" width="3.28515625" customWidth="1"/>
-    <col min="4083" max="4083" width="4.28515625" customWidth="1"/>
-    <col min="4084" max="4120" width="3.28515625" customWidth="1"/>
-    <col min="4329" max="4329" width="20.5703125" customWidth="1"/>
+    <col min="4078" max="4082" width="3.33203125" customWidth="1"/>
+    <col min="4083" max="4083" width="4.33203125" customWidth="1"/>
+    <col min="4084" max="4120" width="3.33203125" customWidth="1"/>
+    <col min="4329" max="4329" width="20.5546875" customWidth="1"/>
     <col min="4330" max="4333" width="0" hidden="1" customWidth="1"/>
-    <col min="4334" max="4338" width="3.28515625" customWidth="1"/>
-    <col min="4339" max="4339" width="4.28515625" customWidth="1"/>
-    <col min="4340" max="4376" width="3.28515625" customWidth="1"/>
-    <col min="4585" max="4585" width="20.5703125" customWidth="1"/>
+    <col min="4334" max="4338" width="3.33203125" customWidth="1"/>
+    <col min="4339" max="4339" width="4.33203125" customWidth="1"/>
+    <col min="4340" max="4376" width="3.33203125" customWidth="1"/>
+    <col min="4585" max="4585" width="20.5546875" customWidth="1"/>
     <col min="4586" max="4589" width="0" hidden="1" customWidth="1"/>
-    <col min="4590" max="4594" width="3.28515625" customWidth="1"/>
-    <col min="4595" max="4595" width="4.28515625" customWidth="1"/>
-    <col min="4596" max="4632" width="3.28515625" customWidth="1"/>
-    <col min="4841" max="4841" width="20.5703125" customWidth="1"/>
+    <col min="4590" max="4594" width="3.33203125" customWidth="1"/>
+    <col min="4595" max="4595" width="4.33203125" customWidth="1"/>
+    <col min="4596" max="4632" width="3.33203125" customWidth="1"/>
+    <col min="4841" max="4841" width="20.5546875" customWidth="1"/>
     <col min="4842" max="4845" width="0" hidden="1" customWidth="1"/>
-    <col min="4846" max="4850" width="3.28515625" customWidth="1"/>
-    <col min="4851" max="4851" width="4.28515625" customWidth="1"/>
-    <col min="4852" max="4888" width="3.28515625" customWidth="1"/>
-    <col min="5097" max="5097" width="20.5703125" customWidth="1"/>
+    <col min="4846" max="4850" width="3.33203125" customWidth="1"/>
+    <col min="4851" max="4851" width="4.33203125" customWidth="1"/>
+    <col min="4852" max="4888" width="3.33203125" customWidth="1"/>
+    <col min="5097" max="5097" width="20.5546875" customWidth="1"/>
     <col min="5098" max="5101" width="0" hidden="1" customWidth="1"/>
-    <col min="5102" max="5106" width="3.28515625" customWidth="1"/>
-    <col min="5107" max="5107" width="4.28515625" customWidth="1"/>
-    <col min="5108" max="5144" width="3.28515625" customWidth="1"/>
-    <col min="5353" max="5353" width="20.5703125" customWidth="1"/>
+    <col min="5102" max="5106" width="3.33203125" customWidth="1"/>
+    <col min="5107" max="5107" width="4.33203125" customWidth="1"/>
+    <col min="5108" max="5144" width="3.33203125" customWidth="1"/>
+    <col min="5353" max="5353" width="20.5546875" customWidth="1"/>
     <col min="5354" max="5357" width="0" hidden="1" customWidth="1"/>
-    <col min="5358" max="5362" width="3.28515625" customWidth="1"/>
-    <col min="5363" max="5363" width="4.28515625" customWidth="1"/>
-    <col min="5364" max="5400" width="3.28515625" customWidth="1"/>
-    <col min="5609" max="5609" width="20.5703125" customWidth="1"/>
+    <col min="5358" max="5362" width="3.33203125" customWidth="1"/>
+    <col min="5363" max="5363" width="4.33203125" customWidth="1"/>
+    <col min="5364" max="5400" width="3.33203125" customWidth="1"/>
+    <col min="5609" max="5609" width="20.5546875" customWidth="1"/>
     <col min="5610" max="5613" width="0" hidden="1" customWidth="1"/>
-    <col min="5614" max="5618" width="3.28515625" customWidth="1"/>
-    <col min="5619" max="5619" width="4.28515625" customWidth="1"/>
-    <col min="5620" max="5656" width="3.28515625" customWidth="1"/>
-    <col min="5865" max="5865" width="20.5703125" customWidth="1"/>
+    <col min="5614" max="5618" width="3.33203125" customWidth="1"/>
+    <col min="5619" max="5619" width="4.33203125" customWidth="1"/>
+    <col min="5620" max="5656" width="3.33203125" customWidth="1"/>
+    <col min="5865" max="5865" width="20.5546875" customWidth="1"/>
     <col min="5866" max="5869" width="0" hidden="1" customWidth="1"/>
-    <col min="5870" max="5874" width="3.28515625" customWidth="1"/>
-    <col min="5875" max="5875" width="4.28515625" customWidth="1"/>
-    <col min="5876" max="5912" width="3.28515625" customWidth="1"/>
-    <col min="6121" max="6121" width="20.5703125" customWidth="1"/>
+    <col min="5870" max="5874" width="3.33203125" customWidth="1"/>
+    <col min="5875" max="5875" width="4.33203125" customWidth="1"/>
+    <col min="5876" max="5912" width="3.33203125" customWidth="1"/>
+    <col min="6121" max="6121" width="20.5546875" customWidth="1"/>
     <col min="6122" max="6125" width="0" hidden="1" customWidth="1"/>
-    <col min="6126" max="6130" width="3.28515625" customWidth="1"/>
-    <col min="6131" max="6131" width="4.28515625" customWidth="1"/>
-    <col min="6132" max="6168" width="3.28515625" customWidth="1"/>
-    <col min="6377" max="6377" width="20.5703125" customWidth="1"/>
+    <col min="6126" max="6130" width="3.33203125" customWidth="1"/>
+    <col min="6131" max="6131" width="4.33203125" customWidth="1"/>
+    <col min="6132" max="6168" width="3.33203125" customWidth="1"/>
+    <col min="6377" max="6377" width="20.5546875" customWidth="1"/>
     <col min="6378" max="6381" width="0" hidden="1" customWidth="1"/>
-    <col min="6382" max="6386" width="3.28515625" customWidth="1"/>
-    <col min="6387" max="6387" width="4.28515625" customWidth="1"/>
-    <col min="6388" max="6424" width="3.28515625" customWidth="1"/>
-    <col min="6633" max="6633" width="20.5703125" customWidth="1"/>
+    <col min="6382" max="6386" width="3.33203125" customWidth="1"/>
+    <col min="6387" max="6387" width="4.33203125" customWidth="1"/>
+    <col min="6388" max="6424" width="3.33203125" customWidth="1"/>
+    <col min="6633" max="6633" width="20.5546875" customWidth="1"/>
     <col min="6634" max="6637" width="0" hidden="1" customWidth="1"/>
-    <col min="6638" max="6642" width="3.28515625" customWidth="1"/>
-    <col min="6643" max="6643" width="4.28515625" customWidth="1"/>
-    <col min="6644" max="6680" width="3.28515625" customWidth="1"/>
-    <col min="6889" max="6889" width="20.5703125" customWidth="1"/>
+    <col min="6638" max="6642" width="3.33203125" customWidth="1"/>
+    <col min="6643" max="6643" width="4.33203125" customWidth="1"/>
+    <col min="6644" max="6680" width="3.33203125" customWidth="1"/>
+    <col min="6889" max="6889" width="20.5546875" customWidth="1"/>
     <col min="6890" max="6893" width="0" hidden="1" customWidth="1"/>
-    <col min="6894" max="6898" width="3.28515625" customWidth="1"/>
-    <col min="6899" max="6899" width="4.28515625" customWidth="1"/>
-    <col min="6900" max="6936" width="3.28515625" customWidth="1"/>
-    <col min="7145" max="7145" width="20.5703125" customWidth="1"/>
+    <col min="6894" max="6898" width="3.33203125" customWidth="1"/>
+    <col min="6899" max="6899" width="4.33203125" customWidth="1"/>
+    <col min="6900" max="6936" width="3.33203125" customWidth="1"/>
+    <col min="7145" max="7145" width="20.5546875" customWidth="1"/>
     <col min="7146" max="7149" width="0" hidden="1" customWidth="1"/>
-    <col min="7150" max="7154" width="3.28515625" customWidth="1"/>
-    <col min="7155" max="7155" width="4.28515625" customWidth="1"/>
-    <col min="7156" max="7192" width="3.28515625" customWidth="1"/>
-    <col min="7401" max="7401" width="20.5703125" customWidth="1"/>
+    <col min="7150" max="7154" width="3.33203125" customWidth="1"/>
+    <col min="7155" max="7155" width="4.33203125" customWidth="1"/>
+    <col min="7156" max="7192" width="3.33203125" customWidth="1"/>
+    <col min="7401" max="7401" width="20.5546875" customWidth="1"/>
     <col min="7402" max="7405" width="0" hidden="1" customWidth="1"/>
-    <col min="7406" max="7410" width="3.28515625" customWidth="1"/>
-    <col min="7411" max="7411" width="4.28515625" customWidth="1"/>
-    <col min="7412" max="7448" width="3.28515625" customWidth="1"/>
-    <col min="7657" max="7657" width="20.5703125" customWidth="1"/>
+    <col min="7406" max="7410" width="3.33203125" customWidth="1"/>
+    <col min="7411" max="7411" width="4.33203125" customWidth="1"/>
+    <col min="7412" max="7448" width="3.33203125" customWidth="1"/>
+    <col min="7657" max="7657" width="20.5546875" customWidth="1"/>
     <col min="7658" max="7661" width="0" hidden="1" customWidth="1"/>
-    <col min="7662" max="7666" width="3.28515625" customWidth="1"/>
-    <col min="7667" max="7667" width="4.28515625" customWidth="1"/>
-    <col min="7668" max="7704" width="3.28515625" customWidth="1"/>
-    <col min="7913" max="7913" width="20.5703125" customWidth="1"/>
+    <col min="7662" max="7666" width="3.33203125" customWidth="1"/>
+    <col min="7667" max="7667" width="4.33203125" customWidth="1"/>
+    <col min="7668" max="7704" width="3.33203125" customWidth="1"/>
+    <col min="7913" max="7913" width="20.5546875" customWidth="1"/>
     <col min="7914" max="7917" width="0" hidden="1" customWidth="1"/>
-    <col min="7918" max="7922" width="3.28515625" customWidth="1"/>
-    <col min="7923" max="7923" width="4.28515625" customWidth="1"/>
-    <col min="7924" max="7960" width="3.28515625" customWidth="1"/>
-    <col min="8169" max="8169" width="20.5703125" customWidth="1"/>
+    <col min="7918" max="7922" width="3.33203125" customWidth="1"/>
+    <col min="7923" max="7923" width="4.33203125" customWidth="1"/>
+    <col min="7924" max="7960" width="3.33203125" customWidth="1"/>
+    <col min="8169" max="8169" width="20.5546875" customWidth="1"/>
     <col min="8170" max="8173" width="0" hidden="1" customWidth="1"/>
-    <col min="8174" max="8178" width="3.28515625" customWidth="1"/>
-    <col min="8179" max="8179" width="4.28515625" customWidth="1"/>
-    <col min="8180" max="8216" width="3.28515625" customWidth="1"/>
-    <col min="8425" max="8425" width="20.5703125" customWidth="1"/>
+    <col min="8174" max="8178" width="3.33203125" customWidth="1"/>
+    <col min="8179" max="8179" width="4.33203125" customWidth="1"/>
+    <col min="8180" max="8216" width="3.33203125" customWidth="1"/>
+    <col min="8425" max="8425" width="20.5546875" customWidth="1"/>
     <col min="8426" max="8429" width="0" hidden="1" customWidth="1"/>
-    <col min="8430" max="8434" width="3.28515625" customWidth="1"/>
-    <col min="8435" max="8435" width="4.28515625" customWidth="1"/>
-    <col min="8436" max="8472" width="3.28515625" customWidth="1"/>
-    <col min="8681" max="8681" width="20.5703125" customWidth="1"/>
+    <col min="8430" max="8434" width="3.33203125" customWidth="1"/>
+    <col min="8435" max="8435" width="4.33203125" customWidth="1"/>
+    <col min="8436" max="8472" width="3.33203125" customWidth="1"/>
+    <col min="8681" max="8681" width="20.5546875" customWidth="1"/>
     <col min="8682" max="8685" width="0" hidden="1" customWidth="1"/>
-    <col min="8686" max="8690" width="3.28515625" customWidth="1"/>
-    <col min="8691" max="8691" width="4.28515625" customWidth="1"/>
-    <col min="8692" max="8728" width="3.28515625" customWidth="1"/>
-    <col min="8937" max="8937" width="20.5703125" customWidth="1"/>
+    <col min="8686" max="8690" width="3.33203125" customWidth="1"/>
+    <col min="8691" max="8691" width="4.33203125" customWidth="1"/>
+    <col min="8692" max="8728" width="3.33203125" customWidth="1"/>
+    <col min="8937" max="8937" width="20.5546875" customWidth="1"/>
     <col min="8938" max="8941" width="0" hidden="1" customWidth="1"/>
-    <col min="8942" max="8946" width="3.28515625" customWidth="1"/>
-    <col min="8947" max="8947" width="4.28515625" customWidth="1"/>
-    <col min="8948" max="8984" width="3.28515625" customWidth="1"/>
-    <col min="9193" max="9193" width="20.5703125" customWidth="1"/>
+    <col min="8942" max="8946" width="3.33203125" customWidth="1"/>
+    <col min="8947" max="8947" width="4.33203125" customWidth="1"/>
+    <col min="8948" max="8984" width="3.33203125" customWidth="1"/>
+    <col min="9193" max="9193" width="20.5546875" customWidth="1"/>
     <col min="9194" max="9197" width="0" hidden="1" customWidth="1"/>
-    <col min="9198" max="9202" width="3.28515625" customWidth="1"/>
-    <col min="9203" max="9203" width="4.28515625" customWidth="1"/>
-    <col min="9204" max="9240" width="3.28515625" customWidth="1"/>
-    <col min="9449" max="9449" width="20.5703125" customWidth="1"/>
+    <col min="9198" max="9202" width="3.33203125" customWidth="1"/>
+    <col min="9203" max="9203" width="4.33203125" customWidth="1"/>
+    <col min="9204" max="9240" width="3.33203125" customWidth="1"/>
+    <col min="9449" max="9449" width="20.5546875" customWidth="1"/>
     <col min="9450" max="9453" width="0" hidden="1" customWidth="1"/>
-    <col min="9454" max="9458" width="3.28515625" customWidth="1"/>
-    <col min="9459" max="9459" width="4.28515625" customWidth="1"/>
-    <col min="9460" max="9496" width="3.28515625" customWidth="1"/>
-    <col min="9705" max="9705" width="20.5703125" customWidth="1"/>
+    <col min="9454" max="9458" width="3.33203125" customWidth="1"/>
+    <col min="9459" max="9459" width="4.33203125" customWidth="1"/>
+    <col min="9460" max="9496" width="3.33203125" customWidth="1"/>
+    <col min="9705" max="9705" width="20.5546875" customWidth="1"/>
     <col min="9706" max="9709" width="0" hidden="1" customWidth="1"/>
-    <col min="9710" max="9714" width="3.28515625" customWidth="1"/>
-    <col min="9715" max="9715" width="4.28515625" customWidth="1"/>
-    <col min="9716" max="9752" width="3.28515625" customWidth="1"/>
-    <col min="9961" max="9961" width="20.5703125" customWidth="1"/>
+    <col min="9710" max="9714" width="3.33203125" customWidth="1"/>
+    <col min="9715" max="9715" width="4.33203125" customWidth="1"/>
+    <col min="9716" max="9752" width="3.33203125" customWidth="1"/>
+    <col min="9961" max="9961" width="20.5546875" customWidth="1"/>
     <col min="9962" max="9965" width="0" hidden="1" customWidth="1"/>
-    <col min="9966" max="9970" width="3.28515625" customWidth="1"/>
-    <col min="9971" max="9971" width="4.28515625" customWidth="1"/>
-    <col min="9972" max="10008" width="3.28515625" customWidth="1"/>
-    <col min="10217" max="10217" width="20.5703125" customWidth="1"/>
+    <col min="9966" max="9970" width="3.33203125" customWidth="1"/>
+    <col min="9971" max="9971" width="4.33203125" customWidth="1"/>
+    <col min="9972" max="10008" width="3.33203125" customWidth="1"/>
+    <col min="10217" max="10217" width="20.5546875" customWidth="1"/>
     <col min="10218" max="10221" width="0" hidden="1" customWidth="1"/>
-    <col min="10222" max="10226" width="3.28515625" customWidth="1"/>
-    <col min="10227" max="10227" width="4.28515625" customWidth="1"/>
-    <col min="10228" max="10264" width="3.28515625" customWidth="1"/>
-    <col min="10473" max="10473" width="20.5703125" customWidth="1"/>
+    <col min="10222" max="10226" width="3.33203125" customWidth="1"/>
+    <col min="10227" max="10227" width="4.33203125" customWidth="1"/>
+    <col min="10228" max="10264" width="3.33203125" customWidth="1"/>
+    <col min="10473" max="10473" width="20.5546875" customWidth="1"/>
     <col min="10474" max="10477" width="0" hidden="1" customWidth="1"/>
-    <col min="10478" max="10482" width="3.28515625" customWidth="1"/>
-    <col min="10483" max="10483" width="4.28515625" customWidth="1"/>
-    <col min="10484" max="10520" width="3.28515625" customWidth="1"/>
-    <col min="10729" max="10729" width="20.5703125" customWidth="1"/>
+    <col min="10478" max="10482" width="3.33203125" customWidth="1"/>
+    <col min="10483" max="10483" width="4.33203125" customWidth="1"/>
+    <col min="10484" max="10520" width="3.33203125" customWidth="1"/>
+    <col min="10729" max="10729" width="20.5546875" customWidth="1"/>
     <col min="10730" max="10733" width="0" hidden="1" customWidth="1"/>
-    <col min="10734" max="10738" width="3.28515625" customWidth="1"/>
-    <col min="10739" max="10739" width="4.28515625" customWidth="1"/>
-    <col min="10740" max="10776" width="3.28515625" customWidth="1"/>
-    <col min="10985" max="10985" width="20.5703125" customWidth="1"/>
+    <col min="10734" max="10738" width="3.33203125" customWidth="1"/>
+    <col min="10739" max="10739" width="4.33203125" customWidth="1"/>
+    <col min="10740" max="10776" width="3.33203125" customWidth="1"/>
+    <col min="10985" max="10985" width="20.5546875" customWidth="1"/>
     <col min="10986" max="10989" width="0" hidden="1" customWidth="1"/>
-    <col min="10990" max="10994" width="3.28515625" customWidth="1"/>
-    <col min="10995" max="10995" width="4.28515625" customWidth="1"/>
-    <col min="10996" max="11032" width="3.28515625" customWidth="1"/>
-    <col min="11241" max="11241" width="20.5703125" customWidth="1"/>
+    <col min="10990" max="10994" width="3.33203125" customWidth="1"/>
+    <col min="10995" max="10995" width="4.33203125" customWidth="1"/>
+    <col min="10996" max="11032" width="3.33203125" customWidth="1"/>
+    <col min="11241" max="11241" width="20.5546875" customWidth="1"/>
     <col min="11242" max="11245" width="0" hidden="1" customWidth="1"/>
-    <col min="11246" max="11250" width="3.28515625" customWidth="1"/>
-    <col min="11251" max="11251" width="4.28515625" customWidth="1"/>
-    <col min="11252" max="11288" width="3.28515625" customWidth="1"/>
-    <col min="11497" max="11497" width="20.5703125" customWidth="1"/>
+    <col min="11246" max="11250" width="3.33203125" customWidth="1"/>
+    <col min="11251" max="11251" width="4.33203125" customWidth="1"/>
+    <col min="11252" max="11288" width="3.33203125" customWidth="1"/>
+    <col min="11497" max="11497" width="20.5546875" customWidth="1"/>
     <col min="11498" max="11501" width="0" hidden="1" customWidth="1"/>
-    <col min="11502" max="11506" width="3.28515625" customWidth="1"/>
-    <col min="11507" max="11507" width="4.28515625" customWidth="1"/>
-    <col min="11508" max="11544" width="3.28515625" customWidth="1"/>
-    <col min="11753" max="11753" width="20.5703125" customWidth="1"/>
+    <col min="11502" max="11506" width="3.33203125" customWidth="1"/>
+    <col min="11507" max="11507" width="4.33203125" customWidth="1"/>
+    <col min="11508" max="11544" width="3.33203125" customWidth="1"/>
+    <col min="11753" max="11753" width="20.5546875" customWidth="1"/>
     <col min="11754" max="11757" width="0" hidden="1" customWidth="1"/>
-    <col min="11758" max="11762" width="3.28515625" customWidth="1"/>
-    <col min="11763" max="11763" width="4.28515625" customWidth="1"/>
-    <col min="11764" max="11800" width="3.28515625" customWidth="1"/>
-    <col min="12009" max="12009" width="20.5703125" customWidth="1"/>
+    <col min="11758" max="11762" width="3.33203125" customWidth="1"/>
+    <col min="11763" max="11763" width="4.33203125" customWidth="1"/>
+    <col min="11764" max="11800" width="3.33203125" customWidth="1"/>
+    <col min="12009" max="12009" width="20.5546875" customWidth="1"/>
     <col min="12010" max="12013" width="0" hidden="1" customWidth="1"/>
-    <col min="12014" max="12018" width="3.28515625" customWidth="1"/>
-    <col min="12019" max="12019" width="4.28515625" customWidth="1"/>
-    <col min="12020" max="12056" width="3.28515625" customWidth="1"/>
-    <col min="12265" max="12265" width="20.5703125" customWidth="1"/>
+    <col min="12014" max="12018" width="3.33203125" customWidth="1"/>
+    <col min="12019" max="12019" width="4.33203125" customWidth="1"/>
+    <col min="12020" max="12056" width="3.33203125" customWidth="1"/>
+    <col min="12265" max="12265" width="20.5546875" customWidth="1"/>
     <col min="12266" max="12269" width="0" hidden="1" customWidth="1"/>
-    <col min="12270" max="12274" width="3.28515625" customWidth="1"/>
-    <col min="12275" max="12275" width="4.28515625" customWidth="1"/>
-    <col min="12276" max="12312" width="3.28515625" customWidth="1"/>
-    <col min="12521" max="12521" width="20.5703125" customWidth="1"/>
+    <col min="12270" max="12274" width="3.33203125" customWidth="1"/>
+    <col min="12275" max="12275" width="4.33203125" customWidth="1"/>
+    <col min="12276" max="12312" width="3.33203125" customWidth="1"/>
+    <col min="12521" max="12521" width="20.5546875" customWidth="1"/>
     <col min="12522" max="12525" width="0" hidden="1" customWidth="1"/>
-    <col min="12526" max="12530" width="3.28515625" customWidth="1"/>
-    <col min="12531" max="12531" width="4.28515625" customWidth="1"/>
-    <col min="12532" max="12568" width="3.28515625" customWidth="1"/>
-    <col min="12777" max="12777" width="20.5703125" customWidth="1"/>
+    <col min="12526" max="12530" width="3.33203125" customWidth="1"/>
+    <col min="12531" max="12531" width="4.33203125" customWidth="1"/>
+    <col min="12532" max="12568" width="3.33203125" customWidth="1"/>
+    <col min="12777" max="12777" width="20.5546875" customWidth="1"/>
     <col min="12778" max="12781" width="0" hidden="1" customWidth="1"/>
-    <col min="12782" max="12786" width="3.28515625" customWidth="1"/>
-    <col min="12787" max="12787" width="4.28515625" customWidth="1"/>
-    <col min="12788" max="12824" width="3.28515625" customWidth="1"/>
-    <col min="13033" max="13033" width="20.5703125" customWidth="1"/>
+    <col min="12782" max="12786" width="3.33203125" customWidth="1"/>
+    <col min="12787" max="12787" width="4.33203125" customWidth="1"/>
+    <col min="12788" max="12824" width="3.33203125" customWidth="1"/>
+    <col min="13033" max="13033" width="20.5546875" customWidth="1"/>
     <col min="13034" max="13037" width="0" hidden="1" customWidth="1"/>
-    <col min="13038" max="13042" width="3.28515625" customWidth="1"/>
-    <col min="13043" max="13043" width="4.28515625" customWidth="1"/>
-    <col min="13044" max="13080" width="3.28515625" customWidth="1"/>
-    <col min="13289" max="13289" width="20.5703125" customWidth="1"/>
+    <col min="13038" max="13042" width="3.33203125" customWidth="1"/>
+    <col min="13043" max="13043" width="4.33203125" customWidth="1"/>
+    <col min="13044" max="13080" width="3.33203125" customWidth="1"/>
+    <col min="13289" max="13289" width="20.5546875" customWidth="1"/>
     <col min="13290" max="13293" width="0" hidden="1" customWidth="1"/>
-    <col min="13294" max="13298" width="3.28515625" customWidth="1"/>
-    <col min="13299" max="13299" width="4.28515625" customWidth="1"/>
-    <col min="13300" max="13336" width="3.28515625" customWidth="1"/>
-    <col min="13545" max="13545" width="20.5703125" customWidth="1"/>
+    <col min="13294" max="13298" width="3.33203125" customWidth="1"/>
+    <col min="13299" max="13299" width="4.33203125" customWidth="1"/>
+    <col min="13300" max="13336" width="3.33203125" customWidth="1"/>
+    <col min="13545" max="13545" width="20.5546875" customWidth="1"/>
     <col min="13546" max="13549" width="0" hidden="1" customWidth="1"/>
-    <col min="13550" max="13554" width="3.28515625" customWidth="1"/>
-    <col min="13555" max="13555" width="4.28515625" customWidth="1"/>
-    <col min="13556" max="13592" width="3.28515625" customWidth="1"/>
-    <col min="13801" max="13801" width="20.5703125" customWidth="1"/>
+    <col min="13550" max="13554" width="3.33203125" customWidth="1"/>
+    <col min="13555" max="13555" width="4.33203125" customWidth="1"/>
+    <col min="13556" max="13592" width="3.33203125" customWidth="1"/>
+    <col min="13801" max="13801" width="20.5546875" customWidth="1"/>
     <col min="13802" max="13805" width="0" hidden="1" customWidth="1"/>
-    <col min="13806" max="13810" width="3.28515625" customWidth="1"/>
-    <col min="13811" max="13811" width="4.28515625" customWidth="1"/>
-    <col min="13812" max="13848" width="3.28515625" customWidth="1"/>
-    <col min="14057" max="14057" width="20.5703125" customWidth="1"/>
+    <col min="13806" max="13810" width="3.33203125" customWidth="1"/>
+    <col min="13811" max="13811" width="4.33203125" customWidth="1"/>
+    <col min="13812" max="13848" width="3.33203125" customWidth="1"/>
+    <col min="14057" max="14057" width="20.5546875" customWidth="1"/>
     <col min="14058" max="14061" width="0" hidden="1" customWidth="1"/>
-    <col min="14062" max="14066" width="3.28515625" customWidth="1"/>
-    <col min="14067" max="14067" width="4.28515625" customWidth="1"/>
-    <col min="14068" max="14104" width="3.28515625" customWidth="1"/>
-    <col min="14313" max="14313" width="20.5703125" customWidth="1"/>
+    <col min="14062" max="14066" width="3.33203125" customWidth="1"/>
+    <col min="14067" max="14067" width="4.33203125" customWidth="1"/>
+    <col min="14068" max="14104" width="3.33203125" customWidth="1"/>
+    <col min="14313" max="14313" width="20.5546875" customWidth="1"/>
     <col min="14314" max="14317" width="0" hidden="1" customWidth="1"/>
-    <col min="14318" max="14322" width="3.28515625" customWidth="1"/>
-    <col min="14323" max="14323" width="4.28515625" customWidth="1"/>
-    <col min="14324" max="14360" width="3.28515625" customWidth="1"/>
-    <col min="14569" max="14569" width="20.5703125" customWidth="1"/>
+    <col min="14318" max="14322" width="3.33203125" customWidth="1"/>
+    <col min="14323" max="14323" width="4.33203125" customWidth="1"/>
+    <col min="14324" max="14360" width="3.33203125" customWidth="1"/>
+    <col min="14569" max="14569" width="20.5546875" customWidth="1"/>
     <col min="14570" max="14573" width="0" hidden="1" customWidth="1"/>
-    <col min="14574" max="14578" width="3.28515625" customWidth="1"/>
-    <col min="14579" max="14579" width="4.28515625" customWidth="1"/>
-    <col min="14580" max="14616" width="3.28515625" customWidth="1"/>
-    <col min="14825" max="14825" width="20.5703125" customWidth="1"/>
+    <col min="14574" max="14578" width="3.33203125" customWidth="1"/>
+    <col min="14579" max="14579" width="4.33203125" customWidth="1"/>
+    <col min="14580" max="14616" width="3.33203125" customWidth="1"/>
+    <col min="14825" max="14825" width="20.5546875" customWidth="1"/>
     <col min="14826" max="14829" width="0" hidden="1" customWidth="1"/>
-    <col min="14830" max="14834" width="3.28515625" customWidth="1"/>
-    <col min="14835" max="14835" width="4.28515625" customWidth="1"/>
-    <col min="14836" max="14872" width="3.28515625" customWidth="1"/>
-    <col min="15081" max="15081" width="20.5703125" customWidth="1"/>
+    <col min="14830" max="14834" width="3.33203125" customWidth="1"/>
+    <col min="14835" max="14835" width="4.33203125" customWidth="1"/>
+    <col min="14836" max="14872" width="3.33203125" customWidth="1"/>
+    <col min="15081" max="15081" width="20.5546875" customWidth="1"/>
     <col min="15082" max="15085" width="0" hidden="1" customWidth="1"/>
-    <col min="15086" max="15090" width="3.28515625" customWidth="1"/>
-    <col min="15091" max="15091" width="4.28515625" customWidth="1"/>
-    <col min="15092" max="15128" width="3.28515625" customWidth="1"/>
-    <col min="15337" max="15337" width="20.5703125" customWidth="1"/>
+    <col min="15086" max="15090" width="3.33203125" customWidth="1"/>
+    <col min="15091" max="15091" width="4.33203125" customWidth="1"/>
+    <col min="15092" max="15128" width="3.33203125" customWidth="1"/>
+    <col min="15337" max="15337" width="20.5546875" customWidth="1"/>
     <col min="15338" max="15341" width="0" hidden="1" customWidth="1"/>
-    <col min="15342" max="15346" width="3.28515625" customWidth="1"/>
-    <col min="15347" max="15347" width="4.28515625" customWidth="1"/>
-    <col min="15348" max="15384" width="3.28515625" customWidth="1"/>
-    <col min="15593" max="15593" width="20.5703125" customWidth="1"/>
+    <col min="15342" max="15346" width="3.33203125" customWidth="1"/>
+    <col min="15347" max="15347" width="4.33203125" customWidth="1"/>
+    <col min="15348" max="15384" width="3.33203125" customWidth="1"/>
+    <col min="15593" max="15593" width="20.5546875" customWidth="1"/>
     <col min="15594" max="15597" width="0" hidden="1" customWidth="1"/>
-    <col min="15598" max="15602" width="3.28515625" customWidth="1"/>
-    <col min="15603" max="15603" width="4.28515625" customWidth="1"/>
-    <col min="15604" max="15640" width="3.28515625" customWidth="1"/>
-    <col min="15849" max="15849" width="20.5703125" customWidth="1"/>
+    <col min="15598" max="15602" width="3.33203125" customWidth="1"/>
+    <col min="15603" max="15603" width="4.33203125" customWidth="1"/>
+    <col min="15604" max="15640" width="3.33203125" customWidth="1"/>
+    <col min="15849" max="15849" width="20.5546875" customWidth="1"/>
     <col min="15850" max="15853" width="0" hidden="1" customWidth="1"/>
-    <col min="15854" max="15858" width="3.28515625" customWidth="1"/>
-    <col min="15859" max="15859" width="4.28515625" customWidth="1"/>
-    <col min="15860" max="15896" width="3.28515625" customWidth="1"/>
-    <col min="16105" max="16105" width="20.5703125" customWidth="1"/>
+    <col min="15854" max="15858" width="3.33203125" customWidth="1"/>
+    <col min="15859" max="15859" width="4.33203125" customWidth="1"/>
+    <col min="15860" max="15896" width="3.33203125" customWidth="1"/>
+    <col min="16105" max="16105" width="20.5546875" customWidth="1"/>
     <col min="16106" max="16109" width="0" hidden="1" customWidth="1"/>
-    <col min="16110" max="16114" width="3.28515625" customWidth="1"/>
-    <col min="16115" max="16115" width="4.28515625" customWidth="1"/>
-    <col min="16116" max="16152" width="3.28515625" customWidth="1"/>
+    <col min="16110" max="16114" width="3.33203125" customWidth="1"/>
+    <col min="16115" max="16115" width="4.33203125" customWidth="1"/>
+    <col min="16116" max="16152" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" thickBot="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:25" ht="23.4" thickBot="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -1321,53 +1320,53 @@
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="60.75" thickBot="1">
-      <c r="A2" s="21"/>
+    <row r="2" spans="1:25" ht="58.2" thickBot="1">
+      <c r="A2" s="22"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="26"/>
     </row>
     <row r="3" spans="1:25" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="22"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="19"/>
     </row>
-    <row r="4" spans="1:25" ht="84.75" thickBot="1">
+    <row r="4" spans="1:25" ht="80.400000000000006" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>60</v>
       </c>
@@ -2233,18 +2232,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65738CFE-501D-41C5-A367-733D105A050C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2878,19 +2877,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE607E6-EB08-40FC-8FB4-901F0E981992}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2911,7 +2910,7 @@
       <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="29" t="str">
+      <c r="C2" s="20" t="str">
         <f>MID(A2, SEARCH("T_",A2,1)+2,99)</f>
         <v>Call</v>
       </c>
@@ -2923,7 +2922,7 @@
       <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="29" t="str">
+      <c r="C3" s="20" t="str">
         <f t="shared" ref="C3:C66" si="0">MID(A3, SEARCH("T_",A3,1)+2,99)</f>
         <v>Telephone_Sales</v>
       </c>
@@ -2935,7 +2934,7 @@
       <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="29" t="str">
+      <c r="C4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campaign_Promotions</v>
       </c>
@@ -2947,7 +2946,7 @@
       <c r="B5" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="29" t="str">
+      <c r="C5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campaign_Record</v>
       </c>
@@ -2959,7 +2958,7 @@
       <c r="B6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="29" t="str">
+      <c r="C6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Collections</v>
       </c>
@@ -2971,7 +2970,7 @@
       <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="29" t="str">
+      <c r="C7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Customer_Service</v>
       </c>
@@ -2983,7 +2982,7 @@
       <c r="B8" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="29" t="str">
+      <c r="C8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Publication</v>
       </c>
@@ -2995,7 +2994,7 @@
       <c r="B9" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="29" t="str">
+      <c r="C9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campus</v>
       </c>
@@ -3007,7 +3006,7 @@
       <c r="B10" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="29" t="str">
+      <c r="C10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Web_Session</v>
       </c>
@@ -3019,7 +3018,7 @@
       <c r="B11" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="29" t="str">
+      <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Prospect_Transaction</v>
       </c>
@@ -3031,7 +3030,7 @@
       <c r="B12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="29" t="str">
+      <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Servicing_Transaction</v>
       </c>
@@ -3043,7 +3042,7 @@
       <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="29" t="str">
+      <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Work_Session</v>
       </c>
@@ -3055,7 +3054,7 @@
       <c r="B14" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="29" t="str">
+      <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Prospect</v>
       </c>
@@ -3067,7 +3066,7 @@
       <c r="B15" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="29" t="str">
+      <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Consolidated_Loans</v>
       </c>
@@ -3079,7 +3078,7 @@
       <c r="B16" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="29" t="str">
+      <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>School_Demographics</v>
       </c>
@@ -3091,7 +3090,7 @@
       <c r="B17" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="29" t="str">
+      <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3103,7 +3102,7 @@
       <c r="B18" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="29" t="str">
+      <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Telephone_Sales</v>
       </c>
@@ -3115,7 +3114,7 @@
       <c r="B19" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="29" t="str">
+      <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3127,7 +3126,7 @@
       <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="29" t="str">
+      <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Interaction</v>
       </c>
@@ -3139,7 +3138,7 @@
       <c r="B21" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="29" t="str">
+      <c r="C21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Call</v>
       </c>
@@ -3151,7 +3150,7 @@
       <c r="B22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="29" t="str">
+      <c r="C22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Telephone_Sales</v>
       </c>
@@ -3163,7 +3162,7 @@
       <c r="B23" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="29" t="str">
+      <c r="C23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campaign_Promotions</v>
       </c>
@@ -3175,7 +3174,7 @@
       <c r="B24" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="29" t="str">
+      <c r="C24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campaign_Record</v>
       </c>
@@ -3187,7 +3186,7 @@
       <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="29" t="str">
+      <c r="C25" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Collections</v>
       </c>
@@ -3199,7 +3198,7 @@
       <c r="B26" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="29" t="str">
+      <c r="C26" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Customer_Service</v>
       </c>
@@ -3211,7 +3210,7 @@
       <c r="B27" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="29" t="str">
+      <c r="C27" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Publication</v>
       </c>
@@ -3223,7 +3222,7 @@
       <c r="B28" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="29" t="str">
+      <c r="C28" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campus</v>
       </c>
@@ -3235,7 +3234,7 @@
       <c r="B29" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="29" t="str">
+      <c r="C29" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Web_Session</v>
       </c>
@@ -3247,7 +3246,7 @@
       <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="29" t="str">
+      <c r="C30" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Prospect_Transaction</v>
       </c>
@@ -3259,7 +3258,7 @@
       <c r="B31" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="29" t="str">
+      <c r="C31" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Servicing_Transaction</v>
       </c>
@@ -3271,7 +3270,7 @@
       <c r="B32" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="29" t="str">
+      <c r="C32" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Work_Session</v>
       </c>
@@ -3283,7 +3282,7 @@
       <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="29" t="str">
+      <c r="C33" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Prospect</v>
       </c>
@@ -3295,7 +3294,7 @@
       <c r="B34" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="29" t="str">
+      <c r="C34" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Consolidated_Loans</v>
       </c>
@@ -3307,7 +3306,7 @@
       <c r="B35" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="29" t="str">
+      <c r="C35" s="20" t="str">
         <f t="shared" si="0"/>
         <v>School_Demographics</v>
       </c>
@@ -3319,7 +3318,7 @@
       <c r="B36" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="29" t="str">
+      <c r="C36" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3331,7 +3330,7 @@
       <c r="B37" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="29" t="str">
+      <c r="C37" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Telephone_Sales</v>
       </c>
@@ -3343,7 +3342,7 @@
       <c r="B38" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="29" t="str">
+      <c r="C38" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3355,7 +3354,7 @@
       <c r="B39" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="29" t="str">
+      <c r="C39" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Interaction</v>
       </c>
@@ -3367,7 +3366,7 @@
       <c r="B40" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="29" t="str">
+      <c r="C40" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Call</v>
       </c>
@@ -3379,7 +3378,7 @@
       <c r="B41" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="29" t="str">
+      <c r="C41" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Telephone_Sales</v>
       </c>
@@ -3391,7 +3390,7 @@
       <c r="B42" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="29" t="str">
+      <c r="C42" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Prospect</v>
       </c>
@@ -3403,7 +3402,7 @@
       <c r="B43" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="29" t="str">
+      <c r="C43" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3415,7 +3414,7 @@
       <c r="B44" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="29" t="str">
+      <c r="C44" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3427,7 +3426,7 @@
       <c r="B45" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="29" t="str">
+      <c r="C45" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3439,7 +3438,7 @@
       <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="29" t="str">
+      <c r="C46" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3451,7 +3450,7 @@
       <c r="B47" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="29" t="str">
+      <c r="C47" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3463,7 +3462,7 @@
       <c r="B48" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="29" t="str">
+      <c r="C48" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3475,7 +3474,7 @@
       <c r="B49" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="29" t="str">
+      <c r="C49" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3487,7 +3486,7 @@
       <c r="B50" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="29" t="str">
+      <c r="C50" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3499,7 +3498,7 @@
       <c r="B51" t="s">
         <v>91</v>
       </c>
-      <c r="C51" s="29" t="str">
+      <c r="C51" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3511,7 +3510,7 @@
       <c r="B52" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="29" t="str">
+      <c r="C52" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3523,7 +3522,7 @@
       <c r="B53" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="29" t="str">
+      <c r="C53" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3535,7 +3534,7 @@
       <c r="B54" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="29" t="str">
+      <c r="C54" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3547,7 +3546,7 @@
       <c r="B55" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="29" t="str">
+      <c r="C55" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3559,7 +3558,7 @@
       <c r="B56" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="29" t="str">
+      <c r="C56" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3571,7 +3570,7 @@
       <c r="B57" t="s">
         <v>93</v>
       </c>
-      <c r="C57" s="29" t="str">
+      <c r="C57" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3583,7 +3582,7 @@
       <c r="B58" t="s">
         <v>93</v>
       </c>
-      <c r="C58" s="29" t="str">
+      <c r="C58" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3595,7 +3594,7 @@
       <c r="B59" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="29" t="str">
+      <c r="C59" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Campus</v>
       </c>
@@ -3607,7 +3606,7 @@
       <c r="B60" t="s">
         <v>93</v>
       </c>
-      <c r="C60" s="29" t="str">
+      <c r="C60" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Web_Session</v>
       </c>
@@ -3619,7 +3618,7 @@
       <c r="B61" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="29" t="str">
+      <c r="C61" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Student</v>
       </c>
@@ -3631,7 +3630,7 @@
       <c r="B62" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="29" t="str">
+      <c r="C62" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Instructor</v>
       </c>
@@ -3643,7 +3642,7 @@
       <c r="B63" t="s">
         <v>94</v>
       </c>
-      <c r="C63" s="29" t="str">
+      <c r="C63" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Work_Session</v>
       </c>
@@ -3655,7 +3654,7 @@
       <c r="B64" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="29" t="str">
+      <c r="C64" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Consolidated_Loans</v>
       </c>
@@ -3667,7 +3666,7 @@
       <c r="B65" t="s">
         <v>94</v>
       </c>
-      <c r="C65" s="29" t="str">
+      <c r="C65" s="20" t="str">
         <f t="shared" si="0"/>
         <v>School_Demographics</v>
       </c>
@@ -3679,7 +3678,7 @@
       <c r="B66" t="s">
         <v>94</v>
       </c>
-      <c r="C66" s="29" t="str">
+      <c r="C66" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Interaction</v>
       </c>
@@ -3691,7 +3690,7 @@
       <c r="B67" t="s">
         <v>95</v>
       </c>
-      <c r="C67" s="29" t="str">
+      <c r="C67" s="20" t="str">
         <f t="shared" ref="C67:C82" si="1">MID(A67, SEARCH("T_",A67,1)+2,99)</f>
         <v>Telephone_Sales</v>
       </c>
@@ -3703,7 +3702,7 @@
       <c r="B68" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="29" t="str">
+      <c r="C68" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Campaign_Promotions</v>
       </c>
@@ -3715,7 +3714,7 @@
       <c r="B69" t="s">
         <v>95</v>
       </c>
-      <c r="C69" s="29" t="str">
+      <c r="C69" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Campaign_Record</v>
       </c>
@@ -3727,7 +3726,7 @@
       <c r="B70" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="29" t="str">
+      <c r="C70" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Prospect_Transaction</v>
       </c>
@@ -3739,7 +3738,7 @@
       <c r="B71" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="29" t="str">
+      <c r="C71" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Prospect</v>
       </c>
@@ -3751,7 +3750,7 @@
       <c r="B72" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="29" t="str">
+      <c r="C72" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3763,7 +3762,7 @@
       <c r="B73" t="s">
         <v>95</v>
       </c>
-      <c r="C73" s="29" t="str">
+      <c r="C73" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Instructor</v>
       </c>
@@ -3775,7 +3774,7 @@
       <c r="B74" t="s">
         <v>96</v>
       </c>
-      <c r="C74" s="29" t="str">
+      <c r="C74" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3787,7 +3786,7 @@
       <c r="B75" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="29" t="str">
+      <c r="C75" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3799,7 +3798,7 @@
       <c r="B76" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="29" t="str">
+      <c r="C76" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3811,7 +3810,7 @@
       <c r="B77" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="29" t="str">
+      <c r="C77" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3823,7 +3822,7 @@
       <c r="B78" t="s">
         <v>100</v>
       </c>
-      <c r="C78" s="29" t="str">
+      <c r="C78" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3835,7 +3834,7 @@
       <c r="B79" t="s">
         <v>99</v>
       </c>
-      <c r="C79" s="29" t="str">
+      <c r="C79" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3847,7 +3846,7 @@
       <c r="B80" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="29" t="str">
+      <c r="C80" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3859,7 +3858,7 @@
       <c r="B81" t="s">
         <v>102</v>
       </c>
-      <c r="C81" s="29" t="str">
+      <c r="C81" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Student</v>
       </c>
@@ -3871,7 +3870,7 @@
       <c r="B82" t="s">
         <v>102</v>
       </c>
-      <c r="C82" s="29" t="str">
+      <c r="C82" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Interaction</v>
       </c>

</xml_diff>